<commit_message>
regen code first draft done
</commit_message>
<xml_diff>
--- a/input/lander_engine.xlsx
+++ b/input/lander_engine.xlsx
@@ -1,128 +1,165 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shortcuts\Documents\GitHub\engine-sizing\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44360622-5CBD-47AD-979D-40A9F7EFA57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9695C18F-395E-4D69-B960-73374E1858F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
     <sheet name="Engine" sheetId="3" r:id="rId2"/>
     <sheet name="Injector" sheetId="2" r:id="rId3"/>
+    <sheet name="Cooling" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="a_c" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="a_c" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="a_c" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="a_c">Definition!#REF!</definedName>
+    <definedName name="a_t" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="a_t" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="a_t" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="a_t">Definition!#REF!</definedName>
+    <definedName name="Ac" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Ac" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Ac" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Ac">Definition!#REF!</definedName>
+    <definedName name="Ae" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Ae" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Ae" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Ae">Definition!#REF!</definedName>
+    <definedName name="Ai" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Ai" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Ai" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Ai">Definition!#REF!</definedName>
+    <definedName name="At" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="At" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="At" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="At">Definition!#REF!</definedName>
+    <definedName name="Cp" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Cp" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Cp" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Cp">Definition!#REF!</definedName>
+    <definedName name="Cv" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Cv" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Cv" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Cv">Definition!#REF!</definedName>
+    <definedName name="e" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="e" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="e" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="e">Definition!#REF!</definedName>
+    <definedName name="ec" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="ec" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="ec" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="ec">Definition!#REF!</definedName>
+    <definedName name="g" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="g" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="g" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="g">Definition!#REF!</definedName>
+    <definedName name="J" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="J" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="J" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="J">Definition!#REF!</definedName>
+    <definedName name="m" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="m" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="m" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="m">Definition!#REF!</definedName>
+    <definedName name="Mc" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Mc" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Mc" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Mc">Definition!#REF!</definedName>
+    <definedName name="Me" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Me" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Me" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Me">Definition!#REF!</definedName>
+    <definedName name="Mi" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Mi" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Mi" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Mi">Definition!#REF!</definedName>
+    <definedName name="Mt" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Mt" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Mt" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Mt">Definition!#REF!</definedName>
+    <definedName name="pc_inj" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="pc_inj" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="pc_inj" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="pc_inj">Definition!#REF!</definedName>
+    <definedName name="pc_ns" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="pc_ns" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="pc_ns" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="pc_ns">Definition!#REF!</definedName>
+    <definedName name="pe" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="pe" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="pe" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="pe">Definition!#REF!</definedName>
+    <definedName name="pi" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="pi" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="pi" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="pi">Definition!#REF!</definedName>
+    <definedName name="pt" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="pt" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="pt" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="pt">Definition!#REF!</definedName>
+    <definedName name="R_" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="R_" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="R_" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="R_">Definition!#REF!</definedName>
+    <definedName name="Tc_ns" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Tc_ns" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Tc_ns" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Tc_ns">Definition!#REF!</definedName>
+    <definedName name="Te" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Te" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Te" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Te">Definition!#REF!</definedName>
+    <definedName name="Ti" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Ti" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Ti" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Ti">Definition!#REF!</definedName>
+    <definedName name="Tt" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Tt" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Tt" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Tt">Definition!#REF!</definedName>
+    <definedName name="v_e" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="v_e" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="v_e" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="v_e">Definition!#REF!</definedName>
+    <definedName name="v_i" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="v_i" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="v_i" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="v_i">Definition!#REF!</definedName>
+    <definedName name="v_inj" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="v_inj" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="v_inj" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="v_inj">Definition!#REF!</definedName>
+    <definedName name="v_t" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="v_t" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="v_t" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="v_t">Definition!#REF!</definedName>
+    <definedName name="Ve" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Ve" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Ve" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Ve">Definition!#REF!</definedName>
+    <definedName name="Vi" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Vi" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Vi" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Vi">Definition!#REF!</definedName>
+    <definedName name="Vt" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="Vt" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="Vt" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="Vt">Definition!#REF!</definedName>
+    <definedName name="w_dot" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="w_dot" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="w_dot" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="w_dot">Definition!#REF!</definedName>
+    <definedName name="y" localSheetId="3">Cooling!#REF!</definedName>
     <definedName name="y" localSheetId="1">Engine!#REF!</definedName>
     <definedName name="y" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="y">Definition!#REF!</definedName>
@@ -147,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="161">
   <si>
     <t>Run Description:</t>
   </si>
@@ -1386,6 +1423,8 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1428,11 +1467,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1500,6 +1537,72 @@
         <a:xfrm>
           <a:off x="902076" y="4968193"/>
           <a:ext cx="4143373" cy="3853076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>621929</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>149664</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2098302</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>58269</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Saturn V F-1 Engine Diagram">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B010E35-45EE-467D-A168-8EE65816E1E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="898154" y="4988364"/>
+          <a:ext cx="4143373" cy="3871005"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1957,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FB38BB-BE64-4050-8878-0E451113B9D1}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1981,24 +2084,24 @@
     <col min="16" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="56" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:15" s="58" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="58" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-    </row>
-    <row r="3" spans="1:15" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
+    <row r="2" spans="1:15" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59"/>
+    </row>
+    <row r="3" spans="1:15" s="62" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
       <c r="E5" s="16"/>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2262,12 +2365,12 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
       <c r="G17" s="13" t="s">
         <v>123</v>
       </c>
@@ -2290,10 +2393,10 @@
       </c>
     </row>
     <row r="18" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
       <c r="G18" s="13" t="s">
         <v>119</v>
       </c>
@@ -2332,18 +2435,18 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
     </row>
     <row r="21" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
       <c r="L21" s="19" t="s">
         <v>53</v>
       </c>
@@ -2375,12 +2478,12 @@
       <c r="M23" s="35"/>
     </row>
     <row r="24" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
       <c r="L24" s="19" t="s">
         <v>52</v>
       </c>
@@ -2390,10 +2493,10 @@
     </row>
     <row r="25" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="22"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="65"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
       <c r="L25" s="13" t="s">
         <v>115</v>
       </c>
@@ -2408,10 +2511,10 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
       <c r="L26" s="25" t="s">
         <v>116</v>
       </c>
@@ -2450,95 +2553,95 @@
       <c r="G28" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H28" s="69" t="s">
+      <c r="H28" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G29" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H29" s="67" t="s">
+      <c r="H29" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="L29" s="54" t="s">
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="L29" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="54"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
     </row>
     <row r="30" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G30" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="H30" s="67" t="s">
+      <c r="H30" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
     </row>
     <row r="31" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G31" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H31" s="67" t="s">
+      <c r="H31" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
     </row>
     <row r="32" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G32" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H32" s="67" t="s">
+      <c r="H32" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="L32" s="54" t="s">
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="L32" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="M32" s="54"/>
-      <c r="N32" s="54"/>
-      <c r="O32" s="54"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
     </row>
     <row r="33" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G33" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="67" t="s">
+      <c r="H33" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
-      <c r="L33" s="54"/>
-      <c r="M33" s="54"/>
-      <c r="N33" s="54"/>
-      <c r="O33" s="54"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
     </row>
     <row r="34" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G34" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H34" s="67" t="s">
+      <c r="H34" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="I34" s="67"/>
-      <c r="J34" s="67"/>
-      <c r="L34" s="54"/>
-      <c r="M34" s="54"/>
-      <c r="N34" s="54"/>
-      <c r="O34" s="54"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
     </row>
     <row r="35" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G35" s="43" t="s">
@@ -2549,16 +2652,16 @@
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="24"/>
-      <c r="L35" s="54"/>
-      <c r="M35" s="54"/>
-      <c r="N35" s="54"/>
-      <c r="O35" s="54"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
     </row>
     <row r="36" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="54"/>
-      <c r="O36" s="54"/>
+      <c r="L36" s="56"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
     </row>
     <row r="37" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G37" s="19" t="s">
@@ -2573,78 +2676,73 @@
       <c r="O37" s="14"/>
     </row>
     <row r="38" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="65" t="s">
+      <c r="B38" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
       <c r="G38" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="69" t="s">
+      <c r="H38" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="I38" s="69"/>
-      <c r="J38" s="69"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
     </row>
     <row r="39" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="66"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
       <c r="G39" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="H39" s="67" t="s">
+      <c r="H39" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="I39" s="67"/>
-      <c r="J39" s="67"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
     </row>
     <row r="40" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="66"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
       <c r="G40" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H40" s="67" t="s">
+      <c r="H40" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="I40" s="67"/>
-      <c r="J40" s="67"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
     </row>
     <row r="41" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G41" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H41" s="67" t="s">
+      <c r="H41" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="I41" s="67"/>
-      <c r="J41" s="67"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
     </row>
     <row r="44" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="61"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
     </row>
     <row r="45" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="H40:J40"/>
     <mergeCell ref="B17:E18"/>
     <mergeCell ref="L32:O34"/>
     <mergeCell ref="A1:XFD3"/>
@@ -2661,6 +2759,11 @@
     <mergeCell ref="H30:J30"/>
     <mergeCell ref="H31:J31"/>
     <mergeCell ref="H32:J32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2672,8 +2775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2558753-C1A4-4F1A-A391-5DC27086ECDF}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2895,4 +2998,719 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882957D3-72BD-4C24-BABD-24012D958910}">
+  <dimension ref="A1:O45"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="22" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11" style="12" customWidth="1"/>
+    <col min="4" max="4" width="7" style="12" customWidth="1"/>
+    <col min="5" max="5" width="41" style="17" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11" style="12" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="45" style="16" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="14" style="15" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="12"/>
+    <col min="15" max="15" width="53.42578125" style="16" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="58" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59"/>
+    </row>
+    <row r="3" spans="1:15" s="62" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61"/>
+    </row>
+    <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="E7" s="16"/>
+      <c r="G7" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
+      <c r="L7" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="30"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="21"/>
+    </row>
+    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="32">
+        <v>550</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="33">
+        <v>220</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
+      <c r="L9" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="33">
+        <v>18</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="N10" s="13"/>
+      <c r="O10" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="34">
+        <v>14.7</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="34">
+        <v>90</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" s="34"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="N12" s="13"/>
+      <c r="O12" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="34">
+        <v>90</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="34">
+        <v>100</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="M13" s="35"/>
+    </row>
+    <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="34">
+        <v>25</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="33">
+        <v>1.3</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M14" s="23"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="21"/>
+    </row>
+    <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="34">
+        <v>40</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="21"/>
+      <c r="L16" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="34">
+        <v>45</v>
+      </c>
+      <c r="N16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="G17" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="34">
+        <v>0</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M17" s="34"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="G18" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" s="34">
+        <v>0</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="M18" s="37">
+        <v>4</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O18" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L19" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19" s="37"/>
+      <c r="N19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O19" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+    </row>
+    <row r="21" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="L21" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="M21" s="23"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="21"/>
+    </row>
+    <row r="22" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L22" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="M22" s="34">
+        <v>80</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="21"/>
+      <c r="M23" s="35"/>
+    </row>
+    <row r="24" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="L24" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M24" s="23"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="21"/>
+    </row>
+    <row r="25" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="22"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="L25" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="M25" s="34">
+        <v>15</v>
+      </c>
+      <c r="N25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="L26" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="M26" s="36">
+        <v>0.25</v>
+      </c>
+      <c r="N26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O26" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="22"/>
+      <c r="G27" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="21"/>
+      <c r="L27" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="M27" s="34">
+        <v>0</v>
+      </c>
+      <c r="N27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O27" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+    </row>
+    <row r="29" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="L29" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+    </row>
+    <row r="30" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+    </row>
+    <row r="31" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+    </row>
+    <row r="32" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="L32" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+    </row>
+    <row r="33" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+    </row>
+    <row r="34" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H34" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
+    </row>
+    <row r="35" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I35" s="13"/>
+      <c r="J35" s="24"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+    </row>
+    <row r="36" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L36" s="56"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+    </row>
+    <row r="37" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="21"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+    </row>
+    <row r="38" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="G38" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+    </row>
+    <row r="39" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="G39" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+    </row>
+    <row r="40" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
+      <c r="G40" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H40" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+    </row>
+    <row r="41" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+    </row>
+    <row r="44" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
+    </row>
+    <row r="45" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="63"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="G44:J45"/>
+    <mergeCell ref="L35:O36"/>
+    <mergeCell ref="B38:E40"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="L29:O30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="L32:O34"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="A1:XFD3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B17:E18"/>
+    <mergeCell ref="G20:J21"/>
+    <mergeCell ref="G24:J26"/>
+    <mergeCell ref="H28:J28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>